<commit_message>
Documentación terminada (Solo falta la evaluación de Daniel)
</commit_message>
<xml_diff>
--- a/Documentación/00 IE Autoevaluación y Coevaluación.xlsx
+++ b/Documentación/00 IE Autoevaluación y Coevaluación.xlsx
@@ -1,20 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26827"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A84627B8-7C32-4595-A756-5112FD73FC8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7433"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Alejandro" sheetId="2" r:id="rId1"/>
+    <sheet name="Daniel" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="122211"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="69">
   <si>
     <t>Conciencia Emocional</t>
   </si>
@@ -226,8 +228,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="10" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="11" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -307,6 +309,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -490,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="34">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -504,7 +514,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -514,6 +524,10 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1" shrinkToFit="1"/>
     </xf>
@@ -541,7 +555,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
@@ -571,10 +585,12 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -609,7 +625,158 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1027" name="AutoShape 3" descr="Image result for inteligencia emocional en la empresa"/>
+        <xdr:cNvPr id="2" name="AutoShape 3" descr="Image result for inteligencia emocional en la empresa">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{947329B2-DFB5-43DF-AEC0-2B6A931BCB14}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="6191250" y="333375"/>
+          <a:ext cx="304800" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="AutoShape 4" descr="Image result for inteligencia emocional en la empresa">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{A7607C9D-B0E1-47BF-BF08-0BE683E5878F}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr>
+          <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvSpPr>
+      </xdr:nvSpPr>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="0" y="571500"/>
+          <a:ext cx="304800" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:extLst>
+          <a:ext uri="{909E8E84-426E-40DD-AFC4-6F175D3DCCD1}">
+            <a14:hiddenFill xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+              <a:solidFill>
+                <a:srgbClr val="FFFFFF"/>
+              </a:solidFill>
+            </a14:hiddenFill>
+          </a:ext>
+        </a:extLst>
+      </xdr:spPr>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>566208</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>141640</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Imagen 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{322B36DD-6957-42E5-A198-E73C3467FDEC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="566208" y="0"/>
+          <a:ext cx="1053042" cy="1770415"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="1027" name="AutoShape 3" descr="Image result for inteligencia emocional en la empresa">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -651,7 +818,13 @@
     </xdr:to>
     <xdr:sp macro="" textlink="">
       <xdr:nvSpPr>
-        <xdr:cNvPr id="1028" name="AutoShape 4" descr="Image result for inteligencia emocional en la empresa"/>
+        <xdr:cNvPr id="1028" name="AutoShape 4" descr="Image result for inteligencia emocional en la empresa">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000004040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvSpPr>
           <a:spLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvSpPr>
@@ -693,7 +866,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="3" name="Imagen 2"/>
+        <xdr:cNvPr id="3" name="Imagen 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000003000000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -720,9 +899,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -760,9 +939,9 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -797,7 +976,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -832,7 +1011,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1005,65 +1184,65 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9109E14C-F749-48F0-9FDC-58E43610613F}">
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:D46"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="D46" sqref="A1:D46"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.19921875" customWidth="1"/>
-    <col min="2" max="2" width="62.33203125" customWidth="1"/>
-    <col min="3" max="3" width="9.3984375" customWidth="1"/>
-    <col min="4" max="4" width="9.6640625" customWidth="1"/>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="25.5" x14ac:dyDescent="0.75">
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
       <c r="B1" s="5" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B2" s="6" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B3" s="6" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="18" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B4" s="6" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B5" s="30" t="s">
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>3</v>
       </c>
-      <c r="B6" s="15"/>
-      <c r="C6" s="12"/>
-      <c r="D6" s="13"/>
-    </row>
-    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="B7" s="29" t="s">
+      <c r="B6" s="17"/>
+      <c r="C6" s="14"/>
+      <c r="D6" s="15"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
         <v>67</v>
       </c>
-      <c r="C7" s="29"/>
-      <c r="D7" s="29"/>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="9"/>
       <c r="B8" s="10"/>
       <c r="C8" s="4" t="s">
@@ -1073,11 +1252,11 @@
         <v>64</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A9" s="25" t="s">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
         <v>49</v>
       </c>
-      <c r="B9" s="25"/>
+      <c r="B9" s="27"/>
       <c r="C9" s="4" t="s">
         <v>65</v>
       </c>
@@ -1085,15 +1264,15 @@
         <v>66</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A10" s="27" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
         <v>51</v>
       </c>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>0</v>
       </c>
@@ -1103,7 +1282,7 @@
       <c r="C11" s="2"/>
       <c r="D11" s="2"/>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>1</v>
       </c>
@@ -1113,7 +1292,7 @@
       <c r="C12" s="2"/>
       <c r="D12" s="2"/>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>2</v>
       </c>
@@ -1123,15 +1302,15 @@
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
     </row>
-    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="11" t="s">
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="B14" s="11"/>
-      <c r="C14" s="11"/>
-      <c r="D14" s="11"/>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>4</v>
       </c>
@@ -1141,7 +1320,7 @@
       <c r="C15" s="2"/>
       <c r="D15" s="2"/>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>5</v>
       </c>
@@ -1151,7 +1330,7 @@
       <c r="C16" s="2"/>
       <c r="D16" s="2"/>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>6</v>
       </c>
@@ -1161,7 +1340,7 @@
       <c r="C17" s="2"/>
       <c r="D17" s="2"/>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>7</v>
       </c>
@@ -1171,7 +1350,7 @@
       <c r="C18" s="2"/>
       <c r="D18" s="2"/>
     </row>
-    <row r="19" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>8</v>
       </c>
@@ -1181,15 +1360,15 @@
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
     </row>
-    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="11" t="s">
+    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="B20" s="11"/>
-      <c r="C20" s="11"/>
-      <c r="D20" s="11"/>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>9</v>
       </c>
@@ -1199,7 +1378,7 @@
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>10</v>
       </c>
@@ -1209,7 +1388,7 @@
       <c r="C22" s="2"/>
       <c r="D22" s="2"/>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>11</v>
       </c>
@@ -1219,7 +1398,7 @@
       <c r="C23" s="2"/>
       <c r="D23" s="2"/>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>12</v>
       </c>
@@ -1229,23 +1408,23 @@
       <c r="C24" s="2"/>
       <c r="D24" s="2"/>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="A25" s="26" t="s">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
         <v>50</v>
       </c>
-      <c r="B25" s="26"/>
+      <c r="B25" s="28"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
     </row>
-    <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="28" t="s">
+    <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
         <v>53</v>
       </c>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-    </row>
-    <row r="27" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>13</v>
       </c>
@@ -1255,7 +1434,7 @@
       <c r="C27" s="2"/>
       <c r="D27" s="2"/>
     </row>
-    <row r="28" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>14</v>
       </c>
@@ -1265,7 +1444,7 @@
       <c r="C28" s="2"/>
       <c r="D28" s="2"/>
     </row>
-    <row r="29" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
@@ -1275,7 +1454,7 @@
       <c r="C29" s="2"/>
       <c r="D29" s="2"/>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>16</v>
       </c>
@@ -1285,7 +1464,7 @@
       <c r="C30" s="2"/>
       <c r="D30" s="2"/>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>17</v>
       </c>
@@ -1295,15 +1474,15 @@
       <c r="C31" s="2"/>
       <c r="D31" s="2"/>
     </row>
-    <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A32" s="11" t="s">
+    <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="B32" s="11"/>
-      <c r="C32" s="11"/>
-      <c r="D32" s="11"/>
-    </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>18</v>
       </c>
@@ -1313,7 +1492,7 @@
       <c r="C33" s="2"/>
       <c r="D33" s="2"/>
     </row>
-    <row r="34" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>19</v>
       </c>
@@ -1323,7 +1502,7 @@
       <c r="C34" s="2"/>
       <c r="D34" s="2"/>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>63</v>
       </c>
@@ -1333,7 +1512,7 @@
       <c r="C35" s="2"/>
       <c r="D35" s="2"/>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>20</v>
       </c>
@@ -1343,7 +1522,7 @@
       <c r="C36" s="2"/>
       <c r="D36" s="2"/>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>21</v>
       </c>
@@ -1353,7 +1532,7 @@
       <c r="C37" s="2"/>
       <c r="D37" s="2"/>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>22</v>
       </c>
@@ -1363,7 +1542,7 @@
       <c r="C38" s="2"/>
       <c r="D38" s="2"/>
     </row>
-    <row r="39" spans="1:4" ht="28.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>45</v>
       </c>
@@ -1373,7 +1552,7 @@
       <c r="C39" s="2"/>
       <c r="D39" s="2"/>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>47</v>
       </c>
@@ -1383,28 +1562,552 @@
       <c r="C40" s="2"/>
       <c r="D40" s="2"/>
     </row>
-    <row r="41" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5"/>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="B42" s="16"/>
-      <c r="C42" s="17"/>
-      <c r="D42" s="18"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="B43" s="19"/>
-      <c r="C43" s="20"/>
-      <c r="D43" s="21"/>
-    </row>
-    <row r="44" spans="1:4" ht="14.65" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="B44" s="22"/>
-      <c r="C44" s="23"/>
-      <c r="D44" s="24"/>
-    </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.45">
-      <c r="C46" s="31"/>
-      <c r="D46" s="31" t="s">
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="24"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="26"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="12"/>
+      <c r="D46" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="11">
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:D26"/>
+    <mergeCell ref="A32:D32"/>
+    <mergeCell ref="B42:D44"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="C6:D6"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A10:D10"/>
+    <mergeCell ref="A14:D14"/>
+  </mergeCells>
+  <pageMargins left="0.70866141732283472" right="0.70866141732283472" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
+  <pageSetup scale="87" orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <sheetPr>
+    <pageSetUpPr fitToPage="1"/>
+  </sheetPr>
+  <dimension ref="A1:D46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6:D6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="62.28515625" customWidth="1"/>
+    <col min="3" max="3" width="9.42578125" customWidth="1"/>
+    <col min="4" max="4" width="9.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="26.25" x14ac:dyDescent="0.4">
+      <c r="B1" s="5" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B2" s="6" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B3" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B4" s="6" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="11" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="17"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+    </row>
+    <row r="7" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="31" t="s">
+        <v>67</v>
+      </c>
+      <c r="C7" s="31"/>
+      <c r="D7" s="31"/>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" s="9"/>
+      <c r="B8" s="10"/>
+      <c r="C8" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B9" s="27"/>
+      <c r="C9" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="D9" s="4" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" s="29" t="s">
+        <v>51</v>
+      </c>
+      <c r="B10" s="29"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="29"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="C11" s="2">
+        <v>2</v>
+      </c>
+      <c r="D11" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A12" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="2">
+        <v>2</v>
+      </c>
+      <c r="D12" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A13" s="8" t="s">
+        <v>2</v>
+      </c>
+      <c r="B13" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="2">
+        <v>2</v>
+      </c>
+      <c r="D13" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="13" t="s">
+        <v>61</v>
+      </c>
+      <c r="B14" s="13"/>
+      <c r="C14" s="13"/>
+      <c r="D14" s="13"/>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A15" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C15" s="2">
+        <v>2</v>
+      </c>
+      <c r="D15" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C16" s="2">
+        <v>2</v>
+      </c>
+      <c r="D16" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A17" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C17" s="2">
+        <v>2</v>
+      </c>
+      <c r="D17" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A18" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="B18" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="C18" s="2">
+        <v>2</v>
+      </c>
+      <c r="D18" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="2">
+        <v>2</v>
+      </c>
+      <c r="D19" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A20" s="13" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="13"/>
+      <c r="C20" s="13"/>
+      <c r="D20" s="13"/>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A21" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="2">
+        <v>2</v>
+      </c>
+      <c r="D21" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A22" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="2">
+        <v>2</v>
+      </c>
+      <c r="D22" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B23" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C23" s="2">
+        <v>2</v>
+      </c>
+      <c r="D23" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C24" s="2">
+        <v>2</v>
+      </c>
+      <c r="D24" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A25" s="28" t="s">
+        <v>50</v>
+      </c>
+      <c r="B25" s="28"/>
+      <c r="C25" s="1"/>
+      <c r="D25" s="1"/>
+    </row>
+    <row r="26" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="B26" s="30"/>
+      <c r="C26" s="30"/>
+      <c r="D26" s="30"/>
+    </row>
+    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="C27" s="2">
+        <v>2</v>
+      </c>
+      <c r="D27" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="B28" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="C28" s="2">
+        <v>2</v>
+      </c>
+      <c r="D28" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="8" t="s">
+        <v>15</v>
+      </c>
+      <c r="B29" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="2">
+        <v>2</v>
+      </c>
+      <c r="D29" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="B30" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="C30" s="2">
+        <v>2</v>
+      </c>
+      <c r="D30" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B31" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="C31" s="2">
+        <v>2</v>
+      </c>
+      <c r="D31" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="13" t="s">
+        <v>57</v>
+      </c>
+      <c r="B32" s="13"/>
+      <c r="C32" s="13"/>
+      <c r="D32" s="13"/>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" s="8" t="s">
+        <v>18</v>
+      </c>
+      <c r="B33" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="C33" s="2">
+        <v>2</v>
+      </c>
+      <c r="D33" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="8" t="s">
+        <v>19</v>
+      </c>
+      <c r="B34" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="C34" s="2">
+        <v>2</v>
+      </c>
+      <c r="D34" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A35" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C35" s="2">
+        <v>2</v>
+      </c>
+      <c r="D35" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A36" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C36" s="2">
+        <v>2</v>
+      </c>
+      <c r="D36" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="8" t="s">
+        <v>21</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="C37" s="2">
+        <v>2</v>
+      </c>
+      <c r="D37" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" s="8" t="s">
+        <v>22</v>
+      </c>
+      <c r="B38" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C38" s="2">
+        <v>2</v>
+      </c>
+      <c r="D38" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="8" t="s">
+        <v>45</v>
+      </c>
+      <c r="B39" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="C39" s="2">
+        <v>2</v>
+      </c>
+      <c r="D39" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B40" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="C40" s="2">
+        <v>2</v>
+      </c>
+      <c r="D40" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A42" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="B42" s="18"/>
+      <c r="C42" s="19"/>
+      <c r="D42" s="20"/>
+    </row>
+    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B43" s="21"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="23"/>
+    </row>
+    <row r="44" spans="1:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="24"/>
+      <c r="C44" s="25"/>
+      <c r="D44" s="26"/>
+    </row>
+    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C46" s="12"/>
+      <c r="D46" s="12" t="s">
         <v>68</v>
       </c>
     </row>

</xml_diff>